<commit_message>
Schema changed. Excels files updated.
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/DisabilityTypes.xlsx
+++ b/DatabaseUpdate/ExcelFiles/DisabilityTypes.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="DisabilityTypes Data" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Data" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -28,64 +28,22 @@
     <x:t>EndDate</x:t>
   </x:si>
   <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Инвалид ВОВ</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Участник ВОВ</x:t>
-  </x:si>
-  <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>Воин-интернационалист</x:t>
+    <x:t>Инвалид I группы</x:t>
   </x:si>
   <x:si>
     <x:t>4</x:t>
   </x:si>
   <x:si>
-    <x:t>Лицо, подвершееся радиационному облучению</x:t>
+    <x:t>Инвалид II группы</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>Лицо, подвергшееся  радиационному облучению в Чернобыле</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Инв. I гр.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Инв. II гр.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Инв. III гр.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ребенок-инвалид</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Инвалид с детства</x:t>
+    <x:t>Инвалид III группы</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -443,7 +401,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D11"/>
+  <x:dimension ref="A1:D4"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -474,7 +432,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D2" s="1">
-        <x:v>2958465</x:v>
+        <x:v>2958100</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:4">
@@ -488,7 +446,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D3" s="1">
-        <x:v>2958465</x:v>
+        <x:v>2958100</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:4">
@@ -502,105 +460,7 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D4" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:4">
-      <x:c r="A5" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C5" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D5" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:4">
-      <x:c r="A6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="C6" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D6" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:4">
-      <x:c r="A7" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C7" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D7" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:4">
-      <x:c r="A8" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="C8" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D8" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:4">
-      <x:c r="A9" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="C9" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D9" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:4">
-      <x:c r="A10" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="C10" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D10" s="1">
-        <x:v>2958465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:4">
-      <x:c r="A11" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C11" s="1">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D11" s="1">
-        <x:v>2958465</x:v>
+        <x:v>2958100</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>